<commit_message>
Aggiornato ObjectID a MagazzionoF
</commit_message>
<xml_diff>
--- a/documentation/Specifiche.xlsx
+++ b/documentation/Specifiche.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andb7\WebstormProjects\apptour\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7A8D4979-B712-4464-8069-278AF0A7697F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F05A1C14-C391-4D78-8800-2E97047001BB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9900" windowHeight="6156" activeTab="1" xr2:uid="{2E08219F-3EE0-4281-A1FC-E99460978121}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="74">
   <si>
     <t>Componente di origine</t>
   </si>
@@ -166,12 +166,6 @@
     <t>magazzinoChild3</t>
   </si>
   <si>
-    <t>magazzinoChild4</t>
-  </si>
-  <si>
-    <t>magazzinoChild5</t>
-  </si>
-  <si>
     <t>viewPreparazione</t>
   </si>
   <si>
@@ -235,7 +229,25 @@
     <t>]</t>
   </si>
   <si>
-    <t>objMApping = [</t>
+    <t>viewMagazzinoF</t>
+  </si>
+  <si>
+    <t>magazzinoFChild1</t>
+  </si>
+  <si>
+    <t>magazzinoFChild2</t>
+  </si>
+  <si>
+    <t>magazzinoFChild3</t>
+  </si>
+  <si>
+    <t>magazzinoFChild4</t>
+  </si>
+  <si>
+    <t>magazzinoFChild5</t>
+  </si>
+  <si>
+    <t>objMapping = [</t>
   </si>
 </sst>
 </file>
@@ -776,10 +788,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C1325FD-EEB6-4A44-9972-1EA265725F37}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -789,10 +801,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -800,7 +812,7 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C9" si="0">A$9</f>
@@ -819,7 +831,7 @@
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="0"/>
@@ -830,7 +842,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F38" si="1">"    ObjectID."&amp;C3 &amp;","</f>
+        <f t="shared" ref="F3:F36" si="1">"    ObjectID."&amp;C3 &amp;","</f>
         <v xml:space="preserve">    ObjectID.viewPiantina,</v>
       </c>
     </row>
@@ -839,14 +851,14 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
         <v>viewPiantina</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E38" si="2">E3+1</f>
+        <f t="shared" ref="E4:E42" si="2">E3+1</f>
         <v>2</v>
       </c>
       <c r="F4" t="str">
@@ -859,7 +871,7 @@
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -879,7 +891,7 @@
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -899,7 +911,7 @@
         <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -919,7 +931,7 @@
         <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -939,7 +951,7 @@
         <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -959,7 +971,7 @@
         <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C10" t="str">
         <f>A15</f>
@@ -979,10 +991,10 @@
         <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C11" t="str">
-        <f>A21</f>
+        <f>A19</f>
         <v>viewPreparazione</v>
       </c>
       <c r="E11">
@@ -999,10 +1011,10 @@
         <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C12" t="str">
-        <f>A27</f>
+        <f>A25</f>
         <v>viewLavorazione</v>
       </c>
       <c r="E12">
@@ -1019,10 +1031,10 @@
         <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C13" t="str">
-        <f>A33</f>
+        <f>A31</f>
         <v>viewFinitura</v>
       </c>
       <c r="E13">
@@ -1039,11 +1051,11 @@
         <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C14" t="str">
-        <f>A$9</f>
-        <v>viewPiantina</v>
+        <f>A37</f>
+        <v>viewMagazzinoF</v>
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
@@ -1051,7 +1063,7 @@
       </c>
       <c r="F14" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    ObjectID.viewPiantina,</v>
+        <v xml:space="preserve">    ObjectID.viewMagazzinoF,</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1059,10 +1071,10 @@
         <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" ref="C15:C38" si="3">A$9</f>
+        <f t="shared" ref="C15:C36" si="3">A$9</f>
         <v>viewPiantina</v>
       </c>
       <c r="E15">
@@ -1079,7 +1091,7 @@
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="3"/>
@@ -1099,7 +1111,7 @@
         <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="3"/>
@@ -1119,7 +1131,7 @@
         <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="3"/>
@@ -1139,7 +1151,7 @@
         <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="3"/>
@@ -1159,7 +1171,7 @@
         <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="3"/>
@@ -1179,7 +1191,7 @@
         <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="3"/>
@@ -1199,7 +1211,7 @@
         <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="3"/>
@@ -1219,7 +1231,7 @@
         <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="3"/>
@@ -1239,7 +1251,7 @@
         <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="3"/>
@@ -1259,7 +1271,7 @@
         <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="3"/>
@@ -1279,7 +1291,7 @@
         <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="3"/>
@@ -1299,7 +1311,7 @@
         <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="3"/>
@@ -1319,7 +1331,7 @@
         <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="3"/>
@@ -1339,7 +1351,7 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="3"/>
@@ -1359,7 +1371,7 @@
         <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="3"/>
@@ -1379,7 +1391,7 @@
         <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="3"/>
@@ -1399,7 +1411,7 @@
         <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="3"/>
@@ -1419,7 +1431,7 @@
         <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="3"/>
@@ -1439,7 +1451,7 @@
         <v>61</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="3"/>
@@ -1459,7 +1471,7 @@
         <v>62</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="3"/>
@@ -1479,7 +1491,7 @@
         <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="3"/>
@@ -1496,13 +1508,13 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C37" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="C37:C42" si="4">A$9</f>
         <v>viewPiantina</v>
       </c>
       <c r="E37">
@@ -1510,19 +1522,19 @@
         <v>35</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F37:F42" si="5">"    ObjectID."&amp;C37 &amp;","</f>
         <v xml:space="preserve">    ObjectID.viewPiantina,</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B38" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C38" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>viewPiantina</v>
       </c>
       <c r="E38">
@@ -1530,13 +1542,93 @@
         <v>36</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">    ObjectID.viewPiantina,</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F39" t="s">
-        <v>68</v>
+      <c r="A39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="4"/>
+        <v>viewPiantina</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">    ObjectID.viewPiantina,</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="4"/>
+        <v>viewPiantina</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">    ObjectID.viewPiantina,</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="4"/>
+        <v>viewPiantina</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">    ObjectID.viewPiantina,</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="4"/>
+        <v>viewPiantina</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">    ObjectID.viewPiantina,</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F43" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ridimensionato per Lenovo E550
</commit_message>
<xml_diff>
--- a/documentation/Specifiche.xlsx
+++ b/documentation/Specifiche.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andb7\WebstormProjects\apptour\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F05A1C14-C391-4D78-8800-2E97047001BB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E69B01F7-3031-491A-81C7-CDCFF7910973}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9900" windowHeight="6156" activeTab="1" xr2:uid="{2E08219F-3EE0-4281-A1FC-E99460978121}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9900" windowHeight="6156" activeTab="2" xr2:uid="{2E08219F-3EE0-4281-A1FC-E99460978121}"/>
   </bookViews>
   <sheets>
     <sheet name="eventi" sheetId="1" r:id="rId1"/>
     <sheet name="objMapping" sheetId="2" r:id="rId2"/>
+    <sheet name="dimensioni" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="80">
   <si>
     <t>Componente di origine</t>
   </si>
@@ -248,6 +249,24 @@
   </si>
   <si>
     <t>objMapping = [</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>bottom</t>
+  </si>
+  <si>
+    <t>view</t>
+  </si>
+  <si>
+    <t>backup</t>
+  </si>
+  <si>
+    <t>piantina</t>
   </si>
 </sst>
 </file>
@@ -790,7 +809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C1325FD-EEB6-4A44-9972-1EA265725F37}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -1635,4 +1654,87 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16DB5FD6-196D-458B-BECE-B0A910CD2DCA}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1">
+        <f t="array" ref="C1">SUM(B2:B4*C2:C4)</f>
+        <v>755</v>
+      </c>
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>80</v>
+      </c>
+      <c r="D2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>90</v>
+      </c>
+      <c r="D3">
+        <v>120</v>
+      </c>
+      <c r="F3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <f>INT(B3*C3/G3)-2</f>
+        <v>58</v>
+      </c>
+      <c r="I3">
+        <f>H3*G3</f>
+        <v>522</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>135</v>
+      </c>
+      <c r="D4">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ridimensionato per Lenovo E550 + specifiche.xlsx
</commit_message>
<xml_diff>
--- a/documentation/Specifiche.xlsx
+++ b/documentation/Specifiche.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andb7\WebstormProjects\apptour\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E69B01F7-3031-491A-81C7-CDCFF7910973}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{03A6BA79-0CD2-4565-A50F-C0FD6561ADD6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9900" windowHeight="6156" activeTab="2" xr2:uid="{2E08219F-3EE0-4281-A1FC-E99460978121}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="84">
   <si>
     <t>Componente di origine</t>
   </si>
@@ -267,13 +267,25 @@
   </si>
   <si>
     <t>piantina</t>
+  </si>
+  <si>
+    <t>magazzino</t>
+  </si>
+  <si>
+    <t>totale</t>
+  </si>
+  <si>
+    <t>num</t>
+  </si>
+  <si>
+    <t>height</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,6 +297,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -331,9 +350,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1658,27 +1681,45 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16DB5FD6-196D-458B-BECE-B0A910CD2DCA}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>74</v>
       </c>
-      <c r="C1">
-        <f t="array" ref="C1">SUM(B2:B4*C2:C4)</f>
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1">
+        <f>SUM(E2:E4)</f>
         <v>755</v>
       </c>
-      <c r="D1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -1688,11 +1729,15 @@
       <c r="C2">
         <v>80</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <f t="array" ref="E2:E4">B2:B4*C2:C4</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -1702,25 +1747,35 @@
       <c r="C3">
         <v>90</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>120</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3">
+        <v>540</v>
+      </c>
+      <c r="G3" t="s">
         <v>79</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>9</v>
       </c>
-      <c r="H3">
-        <f>INT(B3*C3/G3)-2</f>
+      <c r="I3">
+        <f>INT(E3/H3)-2</f>
         <v>58</v>
       </c>
-      <c r="I3">
-        <f>H3*G3</f>
+      <c r="J3">
+        <f>I3*H3</f>
         <v>522</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M3">
+        <f>J3</f>
+        <v>522</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>76</v>
       </c>
@@ -1730,7 +1785,10 @@
       <c r="C4">
         <v>135</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
+        <v>135</v>
+      </c>
+      <c r="E4">
         <v>135</v>
       </c>
     </row>

</xml_diff>